<commit_message>
Correção Gramatical (slide) e Backlog Atualizada na Documentação
</commit_message>
<xml_diff>
--- a/Documentação/backlog-primeira-segunda-sprint.xlsx
+++ b/Documentação/backlog-primeira-segunda-sprint.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>Classificação</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>R26</t>
-  </si>
-  <si>
-    <t>R27</t>
   </si>
   <si>
     <t>Pagina Institucional Nuvem</t>
@@ -275,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,14 +291,8 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -367,30 +358,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -442,12 +409,72 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -457,29 +484,20 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -489,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -504,97 +522,65 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="medium">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -604,36 +590,191 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color auto="1"/>
-        </vertical>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="medium">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -670,12 +811,13 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -697,23 +839,22 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="medium">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top style="medium">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
+        <bottom style="medium">
           <color auto="1"/>
         </bottom>
-        <vertical style="medium">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
+        <vertical/>
+        <horizontal style="medium">
           <color auto="1"/>
         </horizontal>
       </border>
@@ -742,6 +883,50 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -756,13 +941,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A7:D19" totalsRowShown="0" headerRowDxfId="1" dataDxfId="7" headerRowBorderDxfId="2" tableBorderDxfId="6" dataCellStyle="Incorreto">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A7:D19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <autoFilter ref="A7:D19"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Nº do Requisito" dataDxfId="0"/>
-    <tableColumn id="2" name="Requisito" dataDxfId="5"/>
-    <tableColumn id="3" name="Classificação" dataDxfId="3"/>
-    <tableColumn id="4" name="Tamanho" dataDxfId="4"/>
+    <tableColumn id="1" name="Nº do Requisito" dataDxfId="9"/>
+    <tableColumn id="2" name="Requisito" dataDxfId="8"/>
+    <tableColumn id="3" name="Classificação" dataDxfId="7"/>
+    <tableColumn id="4" name="Tamanho" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A20:D34" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A20:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Nº do Requisito" dataDxfId="3"/>
+    <tableColumn id="2" name="Requisito" dataDxfId="2"/>
+    <tableColumn id="3" name="Classificação" dataDxfId="1"/>
+    <tableColumn id="4" name="Tamanho" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1031,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,408 +1296,394 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="7">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="7">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="7">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D22" s="21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D23" s="21">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="8" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D26" s="21">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="19" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="20" t="s">
+      <c r="D27" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D29" s="21">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="11">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="21">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="19" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="20" t="s">
+      <c r="D33" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="10">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="13">
+      <c r="D34" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1507,8 +1691,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>